<commit_message>
Create centralized employee dashboard with usage logs and report statistics - moved from type3.py to main dashboard module
</commit_message>
<xml_diff>
--- a/Report-Generator-IP-main/Automation/backend/certin_vulnerability_format.xlsx
+++ b/Report-Generator-IP-main/Automation/backend/certin_vulnerability_format.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
   <si>
     <t>Asset/Hostname</t>
   </si>
@@ -56,6 +56,9 @@
     <t>Total</t>
   </si>
   <si>
+    <t>Tester_Name</t>
+  </si>
+  <si>
     <t>Observation</t>
   </si>
   <si>
@@ -114,6 +117,9 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>Rohit</t>
   </si>
   <si>
     <t>#1</t>
@@ -180,6 +186,9 @@
   </si>
   <si>
     <t>Network</t>
+  </si>
+  <si>
+    <t>Gaven</t>
   </si>
   <si>
     <t>#2</t>
@@ -833,11 +842,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1372,10 +1381,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
@@ -1385,12 +1394,13 @@
     <col min="6" max="6" width="7" customWidth="1"/>
     <col min="7" max="7" width="4.55555555555556" customWidth="1"/>
     <col min="9" max="9" width="5.87962962962963" customWidth="1"/>
-    <col min="11" max="11" width="6.66666666666667" customWidth="1"/>
-    <col min="12" max="12" width="5.88888888888889" customWidth="1"/>
-    <col min="16" max="16" width="5.44444444444444" customWidth="1"/>
+    <col min="10" max="10" width="14.1296296296296" customWidth="1"/>
+    <col min="12" max="12" width="6.66666666666667" customWidth="1"/>
+    <col min="13" max="13" width="5.88888888888889" customWidth="1"/>
+    <col min="17" max="17" width="5.44444444444444" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1469,16 +1479,19 @@
       <c r="Z1" t="s">
         <v>25</v>
       </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" ht="409.5" spans="1:25">
+    <row r="2" ht="409.5" spans="1:26">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1499,60 +1512,63 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
         <v>3</v>
       </c>
-      <c r="L2" t="s">
-        <v>30</v>
-      </c>
       <c r="M2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2">
+        <v>33</v>
+      </c>
+      <c r="O2" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2">
         <v>8.7</v>
       </c>
-      <c r="P2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="Q2" t="s">
         <v>35</v>
       </c>
+      <c r="R2" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="S2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="T2" t="s">
         <v>38</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="U2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="W2" t="s">
+      <c r="V2" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="W2" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="X2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y2" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="3" ht="409.5" spans="1:24">
+    <row r="3" ht="409.5" spans="1:25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1573,59 +1589,62 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" t="s">
         <v>4</v>
       </c>
-      <c r="L3" t="s">
-        <v>30</v>
-      </c>
       <c r="M3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N3" t="s">
-        <v>46</v>
-      </c>
-      <c r="O3">
+        <v>33</v>
+      </c>
+      <c r="O3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P3">
         <v>7.5</v>
       </c>
-      <c r="P3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R3" t="s">
-        <v>48</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="T3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="R3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" t="s">
         <v>51</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="T3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="W3" t="s">
-        <v>40</v>
+      <c r="U3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="X3" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="https://kandspartners.com"/>
-    <hyperlink ref="Q2" r:id="rId2" display="https://kandspartners.com/get-in-touch/"/>
-    <hyperlink ref="U2" r:id="rId3" display="https://owasp.org/Top10/A07_2021-Identification_and_Authentication_Failures/"/>
-    <hyperlink ref="P3" r:id="rId2" display=" 4.0/AV:N/AC:L/AT:N/PR:N/UI:N/VC:H/VI:N/VA:N/SC:N/SI:N/SA:N"/>
-    <hyperlink ref="Q3" r:id="rId2" display="https://kandspartners.com/get-in-touch/"/>
-    <hyperlink ref="U3" r:id="rId4" display="https://owasp.org/www-community/vulnerabilities/Information_Leakage"/>
+    <hyperlink ref="R2" r:id="rId2" display="https://kandspartners.com/get-in-touch/"/>
+    <hyperlink ref="V2" r:id="rId3" display="https://owasp.org/Top10/A07_2021-Identification_and_Authentication_Failures/"/>
+    <hyperlink ref="Q3" r:id="rId2" display=" 4.0/AV:N/AC:L/AT:N/PR:N/UI:N/VC:H/VI:N/VA:N/SC:N/SI:N/SA:N"/>
+    <hyperlink ref="R3" r:id="rId2" display="https://kandspartners.com/get-in-touch/"/>
+    <hyperlink ref="V3" r:id="rId4" display="https://owasp.org/www-community/vulnerabilities/Information_Leakage"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>